<commit_message>
add report bs ttnm
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateBSTTNM.xlsx
+++ b/ATV_Allowance/Templates/TemplateBSTTNM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Đài Phát thanh - Truyền hình An Giang</t>
   </si>
@@ -77,34 +77,6 @@
     <t>Trưởng phòng</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">BẢNG TỔNG HỢP NHUẬN BÚT PHÁT THANH </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TRỰC TIẾP</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve"> (CTV) </t>
   </si>
   <si>
@@ -121,6 +93,21 @@
   </si>
   <si>
     <t>Bt Duyet</t>
+  </si>
+  <si>
+    <t>DCT</t>
+  </si>
+  <si>
+    <t>KTD</t>
+  </si>
+  <si>
+    <t>TCT</t>
+  </si>
+  <si>
+    <t>KT_TH</t>
+  </si>
+  <si>
+    <t>BẢNG TỔNG HỢP THU LAO BIEN SOAN THONG TIN NGAY MOI</t>
   </si>
 </sst>
 </file>
@@ -131,7 +118,7 @@
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,15 +157,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -188,7 +166,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -250,6 +228,72 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -262,7 +306,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -285,6 +329,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -298,6 +348,39 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -584,10 +667,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,95 +686,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
     </row>
     <row r="2" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="16"/>
+      <c r="J3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14" t="s">
+      <c r="K3" s="16"/>
+      <c r="L3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14" t="s">
+      <c r="M3" s="16"/>
+      <c r="N3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="P3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
@@ -722,17 +805,17 @@
       <c r="M4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="14"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="16"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="13"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -748,63 +831,188 @@
       <c r="P5" s="7"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="P6"/>
-      <c r="Q6" s="8" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="19"/>
+    </row>
+    <row r="7" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="24"/>
+      <c r="H7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="24"/>
+      <c r="J7" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="30"/>
+      <c r="L7" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="25"/>
+      <c r="N7" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="25"/>
+      <c r="P7" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="29"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="16"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="P10"/>
+      <c r="Q10" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="P7"/>
-      <c r="Q7" s="9" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="P11"/>
+      <c r="Q11" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D8"/>
-      <c r="E8" t="s">
+      <c r="D12"/>
+      <c r="E12" t="s">
         <v>14</v>
       </c>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8" t="s">
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12" t="s">
         <v>15</v>
       </c>
-      <c r="M8"/>
-      <c r="P8"/>
-      <c r="Q8" t="s">
+      <c r="M12"/>
+      <c r="P12"/>
+      <c r="Q12" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A2:K2"/>
+  <mergeCells count="27">
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="L7:M8"/>
+    <mergeCell ref="N7:O8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="A1:Q1"/>
@@ -819,6 +1027,7 @@
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="88" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
update deduction in template fix show deduction
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateBSTTNM.xlsx
+++ b/ATV_Allowance/Templates/TemplateBSTTNM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>Đài Phát thanh - Truyền hình An Giang</t>
   </si>
@@ -107,7 +107,10 @@
     <t>KT_TH</t>
   </si>
   <si>
-    <t>BẢNG TỔNG HỢP THU LAO BIEN SOAN THONG TIN NGAY MOI</t>
+    <t>Trừ chỉ tiêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BẢNG TỔNG HỢP THU LAO BIEN SOAN THONG TIN NGAY MOI </t>
   </si>
 </sst>
 </file>
@@ -166,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -295,6 +298,19 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -306,15 +322,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -331,61 +344,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -670,10 +689,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="P3" sqref="P3:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,273 +700,286 @@
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="13" width="4.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="14.5703125" customWidth="1"/>
+    <col min="4" max="14" width="4.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" customWidth="1"/>
+    <col min="16" max="16" width="6.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-    </row>
-    <row r="2" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+    </row>
+    <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+    </row>
+    <row r="3" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="22"/>
+      <c r="N3" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="21"/>
-      <c r="N2" s="32"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-    </row>
-    <row r="3" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="O3" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="32"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="22"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="6"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="11"/>
+    </row>
+    <row r="7" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19" t="s">
+      <c r="D7" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="21"/>
+      <c r="J7" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="27"/>
+      <c r="L7" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="N7" s="22"/>
+      <c r="O7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="20" t="s">
+      <c r="P7" s="24"/>
+      <c r="Q7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="19" t="s">
+      <c r="R7" s="22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="3" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="19"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="23" t="s">
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="22"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="7"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="13"/>
-    </row>
-    <row r="7" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="25"/>
-      <c r="J7" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="30"/>
-      <c r="L7" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="M7" s="27"/>
-      <c r="N7" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" s="27"/>
-      <c r="P7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" s="28"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="19"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
       <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="7"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="6"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
@@ -958,12 +990,13 @@
       <c r="K10"/>
       <c r="L10"/>
       <c r="M10"/>
-      <c r="P10"/>
-      <c r="Q10" s="8" t="s">
+      <c r="N10"/>
+      <c r="Q10"/>
+      <c r="R10" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
@@ -974,13 +1007,14 @@
       <c r="K11"/>
       <c r="L11"/>
       <c r="M11"/>
-      <c r="P11"/>
-      <c r="Q11" s="9" t="s">
+      <c r="N11"/>
+      <c r="Q11"/>
+      <c r="R11" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D12"/>
@@ -997,43 +1031,45 @@
         <v>15</v>
       </c>
       <c r="M12"/>
-      <c r="P12"/>
-      <c r="Q12" t="s">
+      <c r="N12"/>
+      <c r="Q12"/>
+      <c r="R12" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="L7:M8"/>
-    <mergeCell ref="N7:O8"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="A1:Q1"/>
+  <mergeCells count="29">
+    <mergeCell ref="A1:R1"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:N4"/>
     <mergeCell ref="O3:O4"/>
     <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="O7:P8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="88" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add 2 sheets in TS and PT report
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateBSTTNM.xlsx
+++ b/ATV_Allowance/Templates/TemplateBSTTNM.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\ATV-Allowance\ATV-Allowance\ATV_Allowance\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\job\ATV-Allowance\ATV-Allowance\ATV_Allowance\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PV" sheetId="1" r:id="rId1"/>
+    <sheet name="CTV" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="28">
   <si>
     <t>Đài Phát thanh - Truyền hình An Giang</t>
   </si>
@@ -115,21 +116,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -137,7 +138,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -145,7 +146,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -153,7 +154,7 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -317,20 +318,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -340,8 +341,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -370,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -379,15 +380,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -396,33 +430,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -738,119 +745,119 @@
   </sheetPr>
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="27.25" customWidth="1"/>
-    <col min="3" max="3" width="18.125" customWidth="1"/>
-    <col min="4" max="11" width="4.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="11" width="4.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="6" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="4.25" style="1" customWidth="1"/>
-    <col min="15" max="15" width="6.25" customWidth="1"/>
-    <col min="16" max="16" width="6.375" customWidth="1"/>
-    <col min="17" max="17" width="13.125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="14.625" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" customWidth="1"/>
+    <col min="16" max="16" width="6.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:18" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-    </row>
-    <row r="2" spans="1:18" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+    </row>
+    <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-    </row>
-    <row r="3" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+    </row>
+    <row r="3" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26" t="s">
+      <c r="E3" s="30"/>
+      <c r="F3" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26" t="s">
+      <c r="G3" s="30"/>
+      <c r="H3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26" t="s">
+      <c r="I3" s="30"/>
+      <c r="J3" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26" t="s">
+      <c r="K3" s="30"/>
+      <c r="L3" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="26"/>
-      <c r="N3" s="28" t="s">
+      <c r="M3" s="30"/>
+      <c r="N3" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="26" t="s">
+      <c r="O3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="26" t="s">
+      <c r="P3" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="27" t="s">
+      <c r="Q3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="26" t="s">
+      <c r="R3" s="30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="15" t="s">
         <v>7</v>
       </c>
@@ -881,13 +888,13 @@
       <c r="M4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="29"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="26"/>
-    </row>
-    <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="N4" s="40"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="30"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -907,12 +914,12 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="18"/>
     </row>
-    <row r="6" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="31"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -928,7 +935,7 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -947,54 +954,54 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="10"/>
     </row>
-    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="33" t="s">
+      <c r="E8" s="30"/>
+      <c r="F8" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="33" t="s">
+      <c r="G8" s="29"/>
+      <c r="H8" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="34"/>
-      <c r="J8" s="33" t="s">
+      <c r="I8" s="29"/>
+      <c r="J8" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="39"/>
-      <c r="L8" s="26" t="s">
+      <c r="K8" s="35"/>
+      <c r="L8" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="26" t="s">
+      <c r="M8" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="N8" s="26"/>
-      <c r="O8" s="35" t="s">
+      <c r="N8" s="30"/>
+      <c r="O8" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="27" t="s">
+      <c r="P8" s="32"/>
+      <c r="Q8" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="R8" s="26" t="s">
+      <c r="R8" s="30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="15" t="s">
         <v>7</v>
       </c>
@@ -1019,15 +1026,15 @@
       <c r="K9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="26"/>
-    </row>
-    <row r="10" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="30"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
@@ -1047,12 +1054,12 @@
       <c r="Q10" s="22"/>
       <c r="R10" s="18"/>
     </row>
-    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="31"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -1068,12 +1075,12 @@
       <c r="P11" s="11"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12" spans="1:18" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R12" s="24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
@@ -1090,7 +1097,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>11</v>
       </c>
@@ -1116,21 +1123,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="O8:P9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="M8:N9"/>
-    <mergeCell ref="L8:L9"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
@@ -1145,8 +1137,443 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="M8:N9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="O8:P9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:R14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="11" width="4.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" customWidth="1"/>
+    <col min="16" max="16" width="6.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+    </row>
+    <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+    </row>
+    <row r="3" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="30"/>
+      <c r="N3" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="40"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="30"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="18"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="6"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="10"/>
+    </row>
+    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="30"/>
+      <c r="F8" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="29"/>
+      <c r="H8" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="29"/>
+      <c r="J8" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="35"/>
+      <c r="L8" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="30"/>
+      <c r="O8" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="R8" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="30"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="18"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="6"/>
+    </row>
+    <row r="12" spans="1:18" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R12" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="Q13"/>
+      <c r="R13" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="Q14"/>
+      <c r="R14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:N9"/>
+    <mergeCell ref="O8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="88" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add 2 sheet for ttnm, pttt, bsttnm reports
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateBSTTNM.xlsx
+++ b/ATV_Allowance/Templates/TemplateBSTTNM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020"/>
   </bookViews>
   <sheets>
     <sheet name="PV" sheetId="1" r:id="rId1"/>
@@ -320,7 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -359,9 +359,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -386,18 +383,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -413,24 +431,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -745,8 +746,8 @@
   </sheetPr>
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10:R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,100 +765,100 @@
     <col min="18" max="18" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:18" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
     </row>
     <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
     </row>
     <row r="3" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30" t="s">
+      <c r="G3" s="28"/>
+      <c r="H3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30" t="s">
+      <c r="I3" s="28"/>
+      <c r="J3" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30" t="s">
+      <c r="K3" s="28"/>
+      <c r="L3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="30"/>
-      <c r="N3" s="39" t="s">
+      <c r="M3" s="28"/>
+      <c r="N3" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="O3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="36" t="s">
+      <c r="Q3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="30" t="s">
+      <c r="R3" s="28" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="15" t="s">
         <v>7</v>
       </c>
@@ -888,38 +889,38 @@
       <c r="M4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="40"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="30"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="28"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="26"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -934,6 +935,7 @@
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="6"/>
+      <c r="R6" s="42"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -955,53 +957,53 @@
       <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="28" t="s">
+      <c r="E8" s="28"/>
+      <c r="F8" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="28" t="s">
+      <c r="G8" s="36"/>
+      <c r="H8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="28" t="s">
+      <c r="I8" s="36"/>
+      <c r="J8" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="35"/>
-      <c r="L8" s="30" t="s">
+      <c r="K8" s="41"/>
+      <c r="L8" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="30" t="s">
+      <c r="M8" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="N8" s="30"/>
-      <c r="O8" s="31" t="s">
+      <c r="N8" s="28"/>
+      <c r="O8" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="36" t="s">
+      <c r="P8" s="38"/>
+      <c r="Q8" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="R8" s="30" t="s">
+      <c r="R8" s="28" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="15" t="s">
         <v>7</v>
       </c>
@@ -1026,40 +1028,40 @@
       <c r="K9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="30"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="28"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="18"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="26"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -1074,9 +1076,10 @@
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
       <c r="Q11" s="6"/>
-    </row>
-    <row r="12" spans="1:18" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R12" s="24" t="s">
+      <c r="R11" s="42"/>
+    </row>
+    <row r="12" spans="1:18" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R12" s="23" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1123,6 +1126,21 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="O8:P9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="M8:N9"/>
+    <mergeCell ref="L8:L9"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
@@ -1137,21 +1155,6 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="M8:N9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="O8:P9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1165,8 +1168,8 @@
   </sheetPr>
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R11" sqref="R10:R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,162 +1187,162 @@
     <col min="18" max="18" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:18" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
     </row>
     <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
     </row>
     <row r="3" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30" t="s">
+      <c r="G3" s="28"/>
+      <c r="H3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30" t="s">
+      <c r="I3" s="28"/>
+      <c r="J3" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30" t="s">
+      <c r="K3" s="28"/>
+      <c r="L3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="30"/>
-      <c r="N3" s="39" t="s">
+      <c r="M3" s="28"/>
+      <c r="N3" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="O3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="36" t="s">
+      <c r="Q3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="30" t="s">
+      <c r="R3" s="28" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="40"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="30"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="31"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="28"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="18"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="26"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -1354,6 +1357,7 @@
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="6"/>
+      <c r="R6" s="42"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -1375,111 +1379,111 @@
       <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="28" t="s">
+      <c r="E8" s="28"/>
+      <c r="F8" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="28" t="s">
+      <c r="G8" s="36"/>
+      <c r="H8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="28" t="s">
+      <c r="I8" s="36"/>
+      <c r="J8" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="35"/>
-      <c r="L8" s="30" t="s">
+      <c r="K8" s="41"/>
+      <c r="L8" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="30" t="s">
+      <c r="M8" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="N8" s="30"/>
-      <c r="O8" s="31" t="s">
+      <c r="N8" s="28"/>
+      <c r="O8" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="36" t="s">
+      <c r="P8" s="38"/>
+      <c r="Q8" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="R8" s="30" t="s">
+      <c r="R8" s="28" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="30"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="28"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="18"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="26"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -1494,9 +1498,10 @@
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
       <c r="Q11" s="6"/>
-    </row>
-    <row r="12" spans="1:18" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R12" s="24" t="s">
+      <c r="R11" s="42"/>
+    </row>
+    <row r="12" spans="1:18" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R12" s="23" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1543,24 +1548,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:N9"/>
-    <mergeCell ref="O8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A2:R2"/>
@@ -1572,6 +1559,24 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:N9"/>
+    <mergeCell ref="O8:P9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="88" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>